<commit_message>
timber co2 removal is now 1.81kg/kg dry wood
</commit_message>
<xml_diff>
--- a/data/shared/shared_var.xlsx
+++ b/data/shared/shared_var.xlsx
@@ -2455,7 +2455,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10:I16"/>
+      <selection pane="bottomRight" activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2875,7 +2875,7 @@
         <v>dry cleft timber</v>
       </c>
       <c r="G10" s="58">
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H10" s="35">
         <v>55</v>
@@ -2926,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="32" t="s">
         <v>78</v>
       </c>
@@ -2949,14 +2949,14 @@
         <f t="shared" si="3"/>
         <v>dry cleft timber</v>
       </c>
-      <c r="G11" s="132">
-        <v>1.65</v>
+      <c r="G11" s="58">
+        <v>1.81</v>
       </c>
       <c r="H11" s="133">
         <f>H$10</f>
         <v>55</v>
       </c>
-      <c r="I11" s="133">
+      <c r="I11" s="132">
         <f>I$10</f>
         <v>0.32</v>
       </c>
@@ -3011,13 +3011,13 @@
       </c>
       <c r="G12" s="3">
         <f>G11</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H12" s="100">
         <f>H11</f>
         <v>55</v>
       </c>
-      <c r="I12" s="100">
+      <c r="I12" s="121">
         <f>I11</f>
         <v>0.32</v>
       </c>
@@ -3073,13 +3073,13 @@
       </c>
       <c r="G13" s="58">
         <f>G11</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H13" s="129">
         <f>H11</f>
         <v>55</v>
       </c>
-      <c r="I13" s="129">
+      <c r="I13" s="59">
         <f>I11</f>
         <v>0.32</v>
       </c>
@@ -3108,7 +3108,7 @@
       <c r="Q13" s="106"/>
       <c r="R13" s="106"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="53" t="s">
         <v>63</v>
       </c>
@@ -3131,14 +3131,14 @@
         <f t="shared" si="3"/>
         <v>dry cleft timber</v>
       </c>
-      <c r="G14" s="121">
-        <v>1.65</v>
+      <c r="G14" s="58">
+        <v>1.81</v>
       </c>
       <c r="H14" s="133">
         <f>H$10</f>
         <v>55</v>
       </c>
-      <c r="I14" s="133">
+      <c r="I14" s="132">
         <f>I$10</f>
         <v>0.32</v>
       </c>
@@ -3194,13 +3194,13 @@
       </c>
       <c r="G15" s="3">
         <f>G14</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H15" s="100">
         <f>H14</f>
         <v>55</v>
       </c>
-      <c r="I15" s="100">
+      <c r="I15" s="121">
         <f>I14</f>
         <v>0.32</v>
       </c>
@@ -3256,13 +3256,13 @@
       </c>
       <c r="G16" s="58">
         <f>G14</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H16" s="129">
         <f>H14</f>
         <v>55</v>
       </c>
-      <c r="I16" s="129">
+      <c r="I16" s="59">
         <f>I14</f>
         <v>0.32</v>
       </c>
@@ -3291,7 +3291,7 @@
       <c r="Q16" s="106"/>
       <c r="R16" s="106"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="46" t="s">
         <v>64</v>
       </c>
@@ -3314,14 +3314,14 @@
         <f t="shared" si="3"/>
         <v>dry cleft timber</v>
       </c>
-      <c r="G17" s="121">
-        <v>1.65</v>
+      <c r="G17" s="58">
+        <v>1.81</v>
       </c>
       <c r="H17" s="133">
         <f>H$10</f>
         <v>55</v>
       </c>
-      <c r="I17" s="133">
+      <c r="I17" s="132">
         <f>I$10</f>
         <v>0.32</v>
       </c>
@@ -3377,13 +3377,13 @@
       </c>
       <c r="G18" s="3">
         <f>G17</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H18" s="100">
         <f>H17</f>
         <v>55</v>
       </c>
-      <c r="I18" s="100">
+      <c r="I18" s="121">
         <f>I17</f>
         <v>0.32</v>
       </c>
@@ -3439,13 +3439,13 @@
       </c>
       <c r="G19" s="58">
         <f>G17</f>
-        <v>1.65</v>
+        <v>1.81</v>
       </c>
       <c r="H19" s="129">
         <f>H17</f>
         <v>55</v>
       </c>
-      <c r="I19" s="129">
+      <c r="I19" s="59">
         <f>I17</f>
         <v>0.32</v>
       </c>
@@ -3477,7 +3477,7 @@
       <c r="U19" s="29"/>
       <c r="V19" s="29"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>137</v>
       </c>
@@ -3500,8 +3500,8 @@
         <f t="shared" ref="F20" si="6">F10</f>
         <v>dry cleft timber</v>
       </c>
-      <c r="G20" s="121">
-        <v>1.65</v>
+      <c r="G20" s="58">
+        <v>1.81</v>
       </c>
       <c r="H20" s="100"/>
       <c r="I20" s="121"/>
@@ -3759,7 +3759,7 @@
   <dimension ref="A1:R14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3810,7 +3810,7 @@
       <c r="J1" s="128" t="s">
         <v>141</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="130" t="s">
         <v>140</v>
       </c>
       <c r="L1" t="s">
@@ -3855,7 +3855,7 @@
       <c r="J2" s="97" t="s">
         <v>142</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="K2" s="109" t="s">
         <v>144</v>
       </c>
       <c r="L2" s="3" t="s">
@@ -3886,7 +3886,7 @@
       </c>
       <c r="F3" s="130"/>
       <c r="J3" s="34"/>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="130" t="s">
         <v>145</v>
       </c>
     </row>
@@ -4016,7 +4016,12 @@
       <c r="I6" s="27">
         <v>1.81</v>
       </c>
-      <c r="K6" s="108"/>
+      <c r="J6" s="21">
+        <v>55</v>
+      </c>
+      <c r="K6" s="108">
+        <v>0.32</v>
+      </c>
       <c r="L6" s="27">
         <v>0.1918</v>
       </c>
@@ -4070,12 +4075,7 @@
       <c r="I7" s="29">
         <v>1.81</v>
       </c>
-      <c r="J7" s="29">
-        <v>55</v>
-      </c>
-      <c r="K7" s="110">
-        <v>0.32</v>
-      </c>
+      <c r="K7" s="110"/>
       <c r="L7" s="29">
         <f t="shared" si="0"/>
         <v>0.21</v>
@@ -4134,11 +4134,11 @@
         <v>1.81</v>
       </c>
       <c r="J8" s="39">
-        <f>J7</f>
+        <f>J6</f>
         <v>55</v>
       </c>
-      <c r="K8" s="39">
-        <f>K7</f>
+      <c r="K8" s="135">
+        <f>K6</f>
         <v>0.32</v>
       </c>
       <c r="L8" s="33">
@@ -4205,7 +4205,7 @@
         <f>J8</f>
         <v>55</v>
       </c>
-      <c r="K9">
+      <c r="K9" s="108">
         <f>K8</f>
         <v>0.32</v>
       </c>
@@ -4277,7 +4277,7 @@
         <f>J8</f>
         <v>55</v>
       </c>
-      <c r="K10" s="29">
+      <c r="K10" s="110">
         <f>K8</f>
         <v>0.32</v>
       </c>
@@ -4339,11 +4339,11 @@
         <v>1.81</v>
       </c>
       <c r="J11" s="39">
-        <f>J7</f>
+        <f>J6</f>
         <v>55</v>
       </c>
-      <c r="K11" s="39">
-        <f>K7</f>
+      <c r="K11" s="135">
+        <f>K6</f>
         <v>0.32</v>
       </c>
       <c r="L11" s="33">
@@ -4410,7 +4410,7 @@
         <f>J11</f>
         <v>55</v>
       </c>
-      <c r="K12">
+      <c r="K12" s="108">
         <f>K11</f>
         <v>0.32</v>
       </c>
@@ -4482,7 +4482,7 @@
         <f>J11</f>
         <v>55</v>
       </c>
-      <c r="K13" s="29">
+      <c r="K13" s="110">
         <f>K11</f>
         <v>0.32</v>
       </c>
@@ -4526,11 +4526,11 @@
         <v>1.81</v>
       </c>
       <c r="J14">
-        <f>J7</f>
+        <f>J6</f>
         <v>55</v>
       </c>
-      <c r="K14">
-        <f>K7</f>
+      <c r="K14" s="108">
+        <f>K6</f>
         <v>0.32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added shackel 2018 vars
</commit_message>
<xml_diff>
--- a/data/shared/shared_var.xlsx
+++ b/data/shared/shared_var.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="17535" tabRatio="598" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Lime" sheetId="2" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="152">
   <si>
     <t>scenario</t>
   </si>
@@ -604,6 +604,18 @@
   </si>
   <si>
     <t>EU-BAT</t>
+  </si>
+  <si>
+    <t>Solvent Type</t>
+  </si>
+  <si>
+    <t>Schakel-HC</t>
+  </si>
+  <si>
+    <t>MEA</t>
+  </si>
+  <si>
+    <t>CaCO3</t>
   </si>
 </sst>
 </file>
@@ -1745,7 +1757,7 @@
   <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2192,6 +2204,19 @@
       <c r="F20" s="21">
         <f>F4</f>
         <v>2.52E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="C22" s="21">
+        <v>6.0000000000000001E-3</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -2462,7 +2487,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4556,8 +4581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4932,15 +4957,23 @@
       <c r="E23" s="20"/>
     </row>
     <row r="24" spans="1:5" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21"/>
+      <c r="A24" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="B24" s="21"/>
       <c r="C24" s="20"/>
       <c r="D24" s="20"/>
       <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>149</v>
+      </c>
       <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
+      <c r="D25" s="50">
+        <f>180*Ref!B$18</f>
+        <v>0.64800000000000002</v>
+      </c>
       <c r="E25" s="20"/>
     </row>
     <row r="26" spans="1:5" s="21" customFormat="1" x14ac:dyDescent="0.25">
@@ -4997,7 +5030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -5500,15 +5533,15 @@
         <v>136</v>
       </c>
       <c r="C23" s="20">
-        <f>C4</f>
+        <f t="shared" ref="C23:E24" si="2">C4</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D23" s="20">
-        <f>D4</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E23" s="20" t="str">
-        <f>E4</f>
+        <f t="shared" si="2"/>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F23" s="20"/>
@@ -5526,15 +5559,15 @@
         <v>136</v>
       </c>
       <c r="C24" s="20">
-        <f>C5</f>
+        <f t="shared" si="2"/>
         <v>0.56599999999999995</v>
       </c>
       <c r="D24" s="20">
-        <f>D5</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E24" s="20" t="str">
-        <f>E5</f>
+        <f t="shared" si="2"/>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F24" s="20"/>
@@ -6327,13 +6360,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20:G20"/>
+      <selection pane="bottomRight" activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6341,12 +6374,12 @@
     <col min="1" max="1" width="11.28515625" style="21" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="21" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" style="21" customWidth="1"/>
-    <col min="4" max="6" width="8.85546875" style="21"/>
-    <col min="7" max="7" width="8.85546875" style="66"/>
-    <col min="8" max="16384" width="8.85546875" style="21"/>
+    <col min="4" max="7" width="8.85546875" style="21"/>
+    <col min="8" max="8" width="15.5703125" style="66" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="71" t="s">
         <v>43</v>
       </c>
@@ -6366,13 +6399,16 @@
         <v>46</v>
       </c>
       <c r="G1" s="72" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="I1" s="72" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="73" t="s">
         <v>38</v>
       </c>
@@ -6389,12 +6425,13 @@
       <c r="F2" s="75" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="84" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="84" t="s">
         <v>90</v>
       </c>
-      <c r="H2" s="76"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="76"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
@@ -6407,10 +6444,11 @@
       </c>
       <c r="E3" s="76"/>
       <c r="F3" s="76"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="76"/>
-    </row>
-    <row r="4" spans="1:8" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G3" s="76"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="76"/>
+    </row>
+    <row r="4" spans="1:9" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
@@ -6426,12 +6464,13 @@
       <c r="F4" s="80">
         <v>0</v>
       </c>
-      <c r="G4" s="28"/>
-      <c r="H4" s="81" t="s">
+      <c r="G4" s="80"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="81" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>78</v>
       </c>
@@ -6452,13 +6491,16 @@
         <f>3.7667/1.243</f>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H5" s="22">
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="H5" s="75"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="75"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="25" t="s">
         <v>79</v>
       </c>
@@ -6482,12 +6524,16 @@
         <f t="shared" si="0"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G6" s="95">
+      <c r="G6" s="38" t="str">
         <f>G5</f>
+        <v>MEA</v>
+      </c>
+      <c r="H6" s="95">
+        <f>H5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="30" t="s">
         <v>82</v>
       </c>
@@ -6511,12 +6557,16 @@
         <f t="shared" si="1"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G7" s="96">
-        <f>G5</f>
+      <c r="G7" s="38" t="str">
+        <f>G6</f>
+        <v>MEA</v>
+      </c>
+      <c r="H7" s="96">
+        <f>H5</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="60" t="s">
         <v>63</v>
       </c>
@@ -6535,13 +6585,16 @@
       <c r="F8" s="77">
         <v>0</v>
       </c>
-      <c r="G8" s="22">
+      <c r="G8" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H8" s="22">
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="H8" s="78"/>
-    </row>
-    <row r="9" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="78"/>
+    </row>
+    <row r="9" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="52" t="s">
         <v>80</v>
       </c>
@@ -6565,13 +6618,17 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G9" s="95">
+      <c r="G9" s="38" t="str">
         <f>G8</f>
+        <v>MEA</v>
+      </c>
+      <c r="H9" s="95">
+        <f>H8</f>
         <v>1E-3</v>
       </c>
-      <c r="H9" s="21"/>
-    </row>
-    <row r="10" spans="1:8" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9" s="21"/>
+    </row>
+    <row r="10" spans="1:9" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="54" t="s">
         <v>83</v>
       </c>
@@ -6595,12 +6652,16 @@
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G10" s="96">
-        <f>G8</f>
+      <c r="G10" s="38" t="str">
+        <f>G9</f>
+        <v>MEA</v>
+      </c>
+      <c r="H10" s="96">
+        <f>H8</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="53" t="s">
         <v>64</v>
       </c>
@@ -6620,14 +6681,17 @@
       <c r="F11" s="43">
         <v>0</v>
       </c>
-      <c r="G11" s="50">
-        <v>0</v>
-      </c>
-      <c r="H11" s="21" t="s">
+      <c r="G11" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H11" s="50">
+        <v>0</v>
+      </c>
+      <c r="I11" s="21" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
         <v>81</v>
       </c>
@@ -6651,12 +6715,16 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G12" s="49">
+      <c r="G12" s="38" t="str">
         <f>G11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>MEA</v>
+      </c>
+      <c r="H12" s="49">
+        <f>H11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="57" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="54" t="s">
         <v>84</v>
       </c>
@@ -6680,13 +6748,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G13" s="83">
-        <f>G11</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="29"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="38" t="str">
+        <f>G12</f>
+        <v>MEA</v>
+      </c>
+      <c r="H13" s="83">
+        <f>H11</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="29"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
         <v>72</v>
       </c>
@@ -6707,15 +6779,18 @@
         <f>3.7667/1.243</f>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G14" s="22">
+      <c r="G14" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H14" s="22">
         <f>0.001</f>
         <v>1E-3</v>
       </c>
-      <c r="H14" s="75" t="s">
+      <c r="I14" s="75" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="21" t="s">
         <v>73</v>
       </c>
@@ -6739,12 +6814,16 @@
         <f t="shared" si="6"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G15" s="49">
+      <c r="G15" s="38" t="str">
         <f>G14</f>
+        <v>MEA</v>
+      </c>
+      <c r="H15" s="49">
+        <f>H14</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
         <v>74</v>
       </c>
@@ -6768,12 +6847,16 @@
         <f t="shared" si="7"/>
         <v>3.0303298471440061</v>
       </c>
-      <c r="G16" s="83">
-        <f>G14</f>
+      <c r="G16" s="38" t="str">
+        <f>G15</f>
+        <v>MEA</v>
+      </c>
+      <c r="H16" s="83">
+        <f>H14</f>
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>75</v>
       </c>
@@ -6793,14 +6876,17 @@
       <c r="F17" s="43">
         <v>0</v>
       </c>
-      <c r="G17" s="39">
-        <v>0</v>
-      </c>
-      <c r="H17" s="21" t="s">
+      <c r="G17" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H17" s="39">
+        <v>0</v>
+      </c>
+      <c r="I17" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>76</v>
       </c>
@@ -6824,15 +6910,19 @@
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="G18" s="26">
+      <c r="G18" s="38" t="str">
         <f>G17</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="21" t="s">
+        <v>MEA</v>
+      </c>
+      <c r="H18" s="26">
+        <f>H17</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" s="29" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="29" t="s">
         <v>77</v>
       </c>
@@ -6856,15 +6946,19 @@
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="G19" s="58">
-        <f>G17</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="21" t="s">
+      <c r="G19" s="38" t="str">
+        <f>G18</f>
+        <v>MEA</v>
+      </c>
+      <c r="H19" s="58">
+        <f>H17</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="21" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>135</v>
       </c>
@@ -6876,7 +6970,7 @@
         <v>1</v>
       </c>
       <c r="D20" s="21">
-        <f t="shared" ref="D20:G20" si="10">D4</f>
+        <f t="shared" ref="D20:H20" si="10">D4</f>
         <v>0.9</v>
       </c>
       <c r="E20" s="21">
@@ -6887,50 +6981,69 @@
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
-      <c r="G20" s="21">
+      <c r="G20" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="21">
         <f t="shared" si="10"/>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
+    <row r="21" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>147</v>
+      </c>
       <c r="B21" s="21"/>
       <c r="C21" s="21"/>
       <c r="D21" s="21"/>
       <c r="E21" s="21"/>
       <c r="F21" s="21"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="25" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G21" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="H21" s="66"/>
+      <c r="I21" s="21"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="G22" s="21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="21"/>
       <c r="B25" s="21"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
       <c r="E25" s="21"/>
       <c r="F25" s="21"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="21"/>
-    </row>
-    <row r="33" spans="1:8" s="78" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G25" s="21"/>
+      <c r="H25" s="66"/>
+      <c r="I25" s="21"/>
+    </row>
+    <row r="33" spans="1:9" s="78" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="21"/>
       <c r="B33" s="21"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
       <c r="E33" s="21"/>
       <c r="F33" s="21"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="21"/>
-    </row>
-    <row r="37" spans="1:8" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="G33" s="21"/>
+      <c r="H33" s="66"/>
+      <c r="I33" s="21"/>
+    </row>
+    <row r="37" spans="1:9" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="21"/>
       <c r="B37" s="21"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
       <c r="E37" s="21"/>
       <c r="F37" s="21"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7544,10 +7657,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="A20" sqref="A20:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7861,6 +7974,20 @@
         <v>0.32</v>
       </c>
     </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="43">
+        <f>94*Ref!$B$18</f>
+        <v>0.33839999999999998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
bug fixes in factory connections
</commit_message>
<xml_diff>
--- a/data/shared/shared_var.xlsx
+++ b/data/shared/shared_var.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/shared/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14BA20D-18EF-9441-97AA-E0A1555A74D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAF8F39-2562-AB46-A606-544DC2BAE3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="3180" windowWidth="28640" windowHeight="17540" tabRatio="598" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="28640" windowHeight="17540" tabRatio="598" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lime" sheetId="2" r:id="rId1"/>
@@ -224,7 +224,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="739" uniqueCount="180">
   <si>
     <t>scenario</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>km pipeline</t>
+  </si>
+  <si>
+    <t>BBF_IEAGHG</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1096,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1257,6 +1260,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -3705,7 +3709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
@@ -7264,10 +7268,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:K44"/>
+  <dimension ref="A1:K45"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7336,320 +7340,309 @@
         <v>3</v>
       </c>
       <c r="C4" s="20">
-        <f>C8</f>
+        <f>C9</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D4" s="10">
-        <f>D8</f>
-        <v>0.81059390048154101</v>
+        <v>0</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C5" s="68">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D5" s="141">
+        <f>(2.9763+0.6597)/(2.9763+0.6597+0.8496)</f>
+        <v>0.81059390048154101</v>
+      </c>
+      <c r="E5" s="68" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C6" s="20">
         <f>C4</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D5" s="10">
-        <v>0</v>
-      </c>
-      <c r="E5" s="20" t="str">
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="20" t="str">
         <f>E4</f>
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="47">
+      <c r="C7" s="47">
         <f>C4</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D6" s="89">
-        <v>0</v>
-      </c>
-      <c r="E6" s="47" t="str">
+      <c r="D7" s="89">
+        <v>0</v>
+      </c>
+      <c r="E7" s="47" t="str">
         <f>E4</f>
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="41" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+    <row r="8" spans="1:11" s="41" customFormat="1" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="41">
+      <c r="B8" s="29"/>
+      <c r="C8" s="41">
         <f>C4</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D7" s="42">
-        <v>0</v>
-      </c>
-      <c r="E7" s="81" t="str">
+      <c r="D8" s="42">
+        <v>0</v>
+      </c>
+      <c r="E8" s="81" t="str">
         <f>E4</f>
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="32" t="s">
+    <row r="9" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B9" s="32" t="s">
         <v>132</v>
-      </c>
-      <c r="C8" s="61">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D8" s="100">
-        <f>(2.9763+0.6597)/(2.9763+0.6597+0.8496)</f>
-        <v>0.81059390048154101</v>
-      </c>
-      <c r="E8" s="61" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="25" t="s">
-        <v>78</v>
-      </c>
-      <c r="B9" s="25" t="str">
-        <f>B8</f>
-        <v>steel</v>
       </c>
       <c r="C9" s="61">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D9" s="101">
-        <f t="shared" ref="D9" si="0">D$8</f>
-        <v>0.81059390048154101</v>
-      </c>
-      <c r="E9" s="21" t="str">
-        <f>E8</f>
+      <c r="D9" s="100">
+        <v>0</v>
+      </c>
+      <c r="E9" s="61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="25" t="str">
+        <f>B9</f>
+        <v>steel</v>
+      </c>
+      <c r="C10" s="61">
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D10" s="101">
+        <f t="shared" ref="D10" si="0">D$9</f>
+        <v>0</v>
+      </c>
+      <c r="E10" s="21" t="str">
+        <f>E9</f>
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30" t="s">
+    <row r="11" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="30" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="30" t="str">
-        <f>B8</f>
+      <c r="B11" s="30" t="str">
+        <f>B9</f>
         <v>steel</v>
       </c>
-      <c r="C10" s="62">
+      <c r="C11" s="62">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D10" s="102">
-        <f t="shared" ref="D10:E10" si="1">D$8</f>
-        <v>0.81059390048154101</v>
-      </c>
-      <c r="E10" s="41" t="str">
+      <c r="D11" s="102">
+        <f t="shared" ref="D11:E11" si="1">D$9</f>
+        <v>0</v>
+      </c>
+      <c r="E11" s="41" t="str">
         <f t="shared" si="1"/>
         <v>natural gas - IPCC</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="32" t="s">
+    <row r="12" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B12" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C11" s="61">
+      <c r="C12" s="61">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D11" s="100">
-        <v>0</v>
-      </c>
-      <c r="E11" s="61" t="s">
+      <c r="D12" s="100">
+        <v>0</v>
+      </c>
+      <c r="E12" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-    </row>
-    <row r="12" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="51" t="s">
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="51" t="s">
         <v>79</v>
       </c>
-      <c r="B12" s="25" t="str">
-        <f>B11</f>
+      <c r="B13" s="25" t="str">
+        <f>B12</f>
         <v>steel</v>
       </c>
-      <c r="C12" s="20">
-        <f>C11</f>
+      <c r="C13" s="20">
+        <f>C12</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D12" s="101">
-        <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="20" t="str">
-        <f>E11</f>
+      <c r="D13" s="101">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="20" t="str">
+        <f>E12</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="53" t="s">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20"/>
+    </row>
+    <row r="14" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="30" t="str">
-        <f>B11</f>
+      <c r="B14" s="30" t="str">
+        <f>B12</f>
         <v>steel</v>
       </c>
-      <c r="C13" s="41">
-        <f>C11</f>
+      <c r="C14" s="41">
+        <f>C12</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D13" s="102">
-        <f>D11</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="41" t="str">
-        <f>E11</f>
+      <c r="D14" s="102">
+        <f>D12</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="41" t="str">
+        <f>E12</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="41"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-    </row>
-    <row r="14" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="52" t="s">
+      <c r="F14" s="41"/>
+      <c r="G14" s="41"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+    </row>
+    <row r="15" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B15" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C14" s="61">
+      <c r="C15" s="61">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D14" s="100">
-        <v>0</v>
-      </c>
-      <c r="E14" s="61" t="s">
+      <c r="D15" s="100">
+        <v>0</v>
+      </c>
+      <c r="E15" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-    </row>
-    <row r="15" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="46" t="s">
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+    </row>
+    <row r="16" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B15" s="25" t="str">
-        <f>B14</f>
+      <c r="B16" s="25" t="str">
+        <f>B15</f>
         <v>steel</v>
       </c>
-      <c r="C15" s="20">
-        <f>C14</f>
+      <c r="C16" s="20">
+        <f>C15</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D15" s="101">
-        <f>D14</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="20" t="str">
-        <f>E14</f>
+      <c r="D16" s="101">
+        <f>D15</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="20" t="str">
+        <f>E15</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-    </row>
-    <row r="16" spans="1:11" s="56" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="53" t="s">
+      <c r="F16" s="20"/>
+      <c r="G16" s="20"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+    </row>
+    <row r="17" spans="1:11" s="56" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="30" t="str">
-        <f>B14</f>
+      <c r="B17" s="30" t="str">
+        <f>B15</f>
         <v>steel</v>
       </c>
-      <c r="C16" s="41">
-        <f>C14</f>
+      <c r="C17" s="41">
+        <f>C15</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D16" s="102">
-        <f>D14</f>
-        <v>0</v>
-      </c>
-      <c r="E16" s="41" t="str">
-        <f>E14</f>
+      <c r="D17" s="102">
+        <f>D15</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="41" t="str">
+        <f>E15</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="41"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="41"/>
-    </row>
-    <row r="17" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>132</v>
-      </c>
-      <c r="C17" s="61">
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D17" s="100">
-        <v>0</v>
-      </c>
-      <c r="E17" s="61" t="s">
-        <v>59</v>
-      </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
-      <c r="K17" s="20"/>
+      <c r="F17" s="41"/>
+      <c r="G17" s="41"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
     </row>
     <row r="18" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="B18" s="25" t="str">
-        <f>B17</f>
-        <v>steel</v>
-      </c>
-      <c r="C18" s="20">
-        <f>C17</f>
+        <v>71</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="61">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D18" s="101">
-        <f>D17</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="20" t="str">
-        <f>E17</f>
-        <v>natural gas - IPCC</v>
+      <c r="D18" s="100">
+        <v>0</v>
+      </c>
+      <c r="E18" s="61" t="s">
+        <v>59</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="20"/>
@@ -7658,75 +7651,75 @@
       <c r="J18" s="20"/>
       <c r="K18" s="20"/>
     </row>
-    <row r="19" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+    <row r="19" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" s="25" t="str">
+        <f>B18</f>
+        <v>steel</v>
+      </c>
+      <c r="C19" s="20">
+        <f>C18</f>
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D19" s="101">
+        <f>D18</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="20" t="str">
+        <f>E18</f>
+        <v>natural gas - IPCC</v>
+      </c>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
+    </row>
+    <row r="20" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="30" t="str">
-        <f>B17</f>
+      <c r="B20" s="30" t="str">
+        <f>B18</f>
         <v>steel</v>
       </c>
-      <c r="C19" s="41">
-        <f>C17</f>
+      <c r="C20" s="41">
+        <f>C18</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D19" s="102">
-        <f>D17</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="41" t="str">
-        <f>E17</f>
+      <c r="D20" s="102">
+        <f>D18</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="41" t="str">
+        <f>E18</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="41"/>
-    </row>
-    <row r="20" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+    </row>
+    <row r="21" spans="1:11" s="39" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B21" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C20" s="61">
+      <c r="C21" s="61">
         <v>0.56599999999999995</v>
       </c>
-      <c r="D20" s="100">
-        <v>0</v>
-      </c>
-      <c r="E20" s="61" t="s">
+      <c r="D21" s="100">
+        <v>0</v>
+      </c>
+      <c r="E21" s="61" t="s">
         <v>59</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-    </row>
-    <row r="21" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" s="25" t="str">
-        <f>B20</f>
-        <v>steel</v>
-      </c>
-      <c r="C21" s="20">
-        <f>C20</f>
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D21" s="101">
-        <f>D20</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="20" t="str">
-        <f>E20</f>
-        <v>natural gas - IPCC</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="20"/>
@@ -7735,75 +7728,76 @@
       <c r="J21" s="20"/>
       <c r="K21" s="20"/>
     </row>
-    <row r="22" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+    <row r="22" spans="1:11" s="21" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B22" s="25" t="str">
+        <f>B21</f>
+        <v>steel</v>
+      </c>
+      <c r="C22" s="20">
+        <f>C21</f>
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D22" s="101">
+        <f>D21</f>
+        <v>0</v>
+      </c>
+      <c r="E22" s="20" t="str">
+        <f>E21</f>
+        <v>natural gas - IPCC</v>
+      </c>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+    </row>
+    <row r="23" spans="1:11" s="29" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="B22" s="30" t="str">
-        <f>B20</f>
+      <c r="B23" s="30" t="str">
+        <f>B21</f>
         <v>steel</v>
       </c>
-      <c r="C22" s="41">
-        <f>C20</f>
+      <c r="C23" s="41">
+        <f>C21</f>
         <v>0.56599999999999995</v>
       </c>
-      <c r="D22" s="102">
-        <f>D20</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="41" t="str">
-        <f>E20</f>
+      <c r="D23" s="102">
+        <f>D21</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="41" t="str">
+        <f>E21</f>
         <v>natural gas - IPCC</v>
       </c>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="41"/>
-    </row>
-    <row r="23" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="F23" s="41"/>
+      <c r="G23" s="41"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
+      <c r="J23" s="41"/>
+      <c r="K23" s="41"/>
+    </row>
+    <row r="24" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>133</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="C23" s="20">
-        <f t="shared" ref="C23:E26" si="2">C4</f>
-        <v>0.56599999999999995</v>
-      </c>
-      <c r="D23" s="20">
-        <v>0</v>
-      </c>
-      <c r="E23" s="20" t="str">
-        <f t="shared" si="2"/>
-        <v>natural gas - IPCC</v>
-      </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
-    </row>
-    <row r="24" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21" t="s">
-        <v>145</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>134</v>
       </c>
       <c r="C24" s="20">
-        <f t="shared" si="2"/>
+        <f>C4</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D24" s="20">
-        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="E24" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>E4</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F24" s="20"/>
@@ -7813,23 +7807,23 @@
       <c r="J24" s="20"/>
       <c r="K24" s="20"/>
     </row>
-    <row r="25" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27" t="s">
-        <v>148</v>
+    <row r="25" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
+        <v>145</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="C25" s="21">
-        <f>C4</f>
+      <c r="C25" s="20">
+        <f>C6</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D25" s="20">
-        <f t="shared" si="2"/>
+        <f>D6</f>
         <v>0</v>
       </c>
       <c r="E25" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>E6</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F25" s="20"/>
@@ -7841,21 +7835,21 @@
     </row>
     <row r="26" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>134</v>
       </c>
       <c r="C26" s="21">
-        <f>C5</f>
+        <f>C4</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D26" s="20">
-        <f t="shared" si="2"/>
+        <f>D7</f>
         <v>0</v>
       </c>
       <c r="E26" s="20" t="str">
-        <f t="shared" si="2"/>
+        <f>E7</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F26" s="20"/>
@@ -7867,20 +7861,22 @@
     </row>
     <row r="27" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
-        <v>161</v>
-      </c>
-      <c r="B27" s="27" t="s">
-        <v>162</v>
+        <v>149</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="C27" s="21">
         <f>C6</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D27" s="20">
-        <v>1</v>
-      </c>
-      <c r="E27" s="47" t="s">
-        <v>166</v>
+        <f t="shared" ref="D27:E27" si="2">D8</f>
+        <v>0</v>
+      </c>
+      <c r="E27" s="20" t="str">
+        <f t="shared" si="2"/>
+        <v>natural gas - IPCC</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="20"/>
@@ -7889,23 +7885,22 @@
       <c r="J27" s="20"/>
       <c r="K27" s="20"/>
     </row>
-    <row r="28" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
-        <v>171</v>
-      </c>
-      <c r="B28" s="21" t="s">
-        <v>134</v>
+        <v>161</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>162</v>
       </c>
       <c r="C28" s="21">
-        <f t="shared" ref="C28:C31" si="3">C7</f>
+        <f>C7</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D28" s="20">
-        <v>0</v>
-      </c>
-      <c r="E28" s="20" t="str">
-        <f t="shared" ref="E28" si="4">E9</f>
-        <v>natural gas - IPCC</v>
+        <v>1</v>
+      </c>
+      <c r="E28" s="47" t="s">
+        <v>166</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
@@ -7914,22 +7909,22 @@
       <c r="J28" s="20"/>
       <c r="K28" s="20"/>
     </row>
-    <row r="29" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B29" s="21" t="s">
         <v>134</v>
       </c>
       <c r="C29" s="21">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C29:C32" si="3">C8</f>
         <v>0.56599999999999995</v>
       </c>
       <c r="D29" s="20">
         <v>0</v>
       </c>
       <c r="E29" s="20" t="str">
-        <f t="shared" ref="E29" si="5">E10</f>
+        <f t="shared" ref="E29" si="4">E10</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F29" s="20"/>
@@ -7941,20 +7936,20 @@
     </row>
     <row r="30" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
-        <v>173</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>162</v>
+        <v>172</v>
+      </c>
+      <c r="B30" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="C30" s="21">
         <f t="shared" si="3"/>
         <v>0.56599999999999995</v>
       </c>
       <c r="D30" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="20" t="str">
-        <f t="shared" ref="E30" si="6">E11</f>
+        <f t="shared" ref="E30" si="5">E11</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F30" s="20"/>
@@ -7966,7 +7961,7 @@
     </row>
     <row r="31" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>162</v>
@@ -7979,7 +7974,7 @@
         <v>1</v>
       </c>
       <c r="E31" s="20" t="str">
-        <f t="shared" ref="E31" si="7">E12</f>
+        <f t="shared" ref="E31" si="6">E12</f>
         <v>natural gas - IPCC</v>
       </c>
       <c r="F31" s="20"/>
@@ -7989,12 +7984,24 @@
       <c r="J31" s="20"/>
       <c r="K31" s="20"/>
     </row>
-    <row r="32" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
+    <row r="32" spans="1:11" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="21">
+        <f t="shared" si="3"/>
+        <v>0.56599999999999995</v>
+      </c>
+      <c r="D32" s="20">
+        <v>1</v>
+      </c>
+      <c r="E32" s="20" t="str">
+        <f t="shared" ref="E32" si="7">E13</f>
+        <v>natural gas - IPCC</v>
+      </c>
       <c r="F32" s="20"/>
       <c r="G32" s="20"/>
       <c r="H32" s="20"/>
@@ -8002,46 +8009,59 @@
       <c r="J32" s="20"/>
       <c r="K32" s="20"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
-      <c r="G36" s="20"/>
-      <c r="H36" s="20"/>
-      <c r="I36" s="20"/>
-      <c r="J36" s="20"/>
-      <c r="K36" s="20"/>
-    </row>
-    <row r="40" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-    </row>
-    <row r="42" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="21"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
-      <c r="K44" s="20"/>
+    <row r="33" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+    </row>
+    <row r="35" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="20"/>
+      <c r="I37" s="20"/>
+      <c r="J37" s="20"/>
+      <c r="K37" s="20"/>
+    </row>
+    <row r="41" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
+      <c r="G41" s="20"/>
+      <c r="H41" s="20"/>
+      <c r="I41" s="20"/>
+      <c r="J41" s="20"/>
+      <c r="K41" s="20"/>
+    </row>
+    <row r="43" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:11" s="61" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="20"/>
+      <c r="J45" s="20"/>
+      <c r="K45" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>